<commit_message>
Updates ontorat and Ontofox fiiles
Updates ontorat and Ontofox fiiles:
- ontofox updates of pr and chebi imports
- Changed Shah's previous drugbank ontorat output file name.
- Updated Du's drugbank ontorat input and output files.
</commit_message>
<xml_diff>
--- a/src/ontology/Ontorat input/Jinyang Du Ontorat/Du_reorganized_data.xlsx
+++ b/src/ontology/Ontorat input/Jinyang Du Ontorat/Du_reorganized_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C4FAD-C912-7B43-B4D6-9AD1000A8753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA1BCC-5582-3543-93B7-071CFBF2FAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Sheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="363">
   <si>
     <t>Drug Label</t>
   </si>
@@ -695,12 +695,6 @@
     <t>antagonist</t>
   </si>
   <si>
-    <t>4E1Rcat</t>
-  </si>
-  <si>
-    <t>may make worse?</t>
-  </si>
-  <si>
     <t>CHEBI_9168</t>
   </si>
   <si>
@@ -725,19 +719,7 @@
     <t>chemical has protein target as agonist</t>
   </si>
   <si>
-    <t>NCIT_C61559</t>
-  </si>
-  <si>
-    <t>degradation</t>
-  </si>
-  <si>
     <t>chemical binds protein</t>
-  </si>
-  <si>
-    <t>translational initiation</t>
-  </si>
-  <si>
-    <t>GO_0006413</t>
   </si>
   <si>
     <t>CHEBI_138090 </t>
@@ -1133,10 +1115,13 @@
     <t>CHEBI_91796</t>
   </si>
   <si>
-    <t>CHEBI_125598</t>
+    <t>Role Label</t>
   </si>
   <si>
-    <t>Role Label</t>
+    <t>CIDO_0000045</t>
+  </si>
+  <si>
+    <t>chemical degrades protein</t>
   </si>
 </sst>
 </file>
@@ -1497,11 +1482,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1050"/>
+  <dimension ref="A1:AC1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="134" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1524,10 +1509,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1587,19 +1572,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>14</v>
@@ -1612,7 +1597,7 @@
         <v>16</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>17</v>
@@ -1644,19 +1629,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>22</v>
@@ -1669,7 +1654,7 @@
         <v>24</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>17</v>
@@ -1701,19 +1686,19 @@
         <v>19</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>22</v>
@@ -1726,7 +1711,7 @@
         <v>25</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>17</v>
@@ -1758,19 +1743,19 @@
         <v>19</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>22</v>
@@ -1807,19 +1792,19 @@
         <v>27</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>22</v>
@@ -1832,7 +1817,7 @@
         <v>30</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>17</v>
@@ -1864,19 +1849,19 @@
         <v>31</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>22</v>
@@ -1889,7 +1874,7 @@
         <v>34</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>17</v>
@@ -1921,19 +1906,19 @@
         <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>22</v>
@@ -1948,7 +1933,7 @@
         <v>39</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>17</v>
@@ -1984,32 +1969,32 @@
         <v>40</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>17</v>
@@ -2043,32 +2028,32 @@
         <v>40</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>17</v>
@@ -2102,25 +2087,25 @@
         <v>40</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="5"/>
@@ -2153,19 +2138,19 @@
         <v>45</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>14</v>
@@ -2178,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>17</v>
@@ -2210,19 +2195,19 @@
         <v>45</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>14</v>
@@ -2235,7 +2220,7 @@
         <v>16</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>17</v>
@@ -2267,19 +2252,19 @@
         <v>45</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>14</v>
@@ -2316,19 +2301,19 @@
         <v>48</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>22</v>
@@ -2341,7 +2326,7 @@
         <v>16</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>17</v>
@@ -2373,19 +2358,19 @@
         <v>51</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>22</v>
@@ -2400,7 +2385,7 @@
         <v>55</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>17</v>
@@ -2432,19 +2417,19 @@
         <v>51</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>22</v>
@@ -2459,7 +2444,7 @@
         <v>55</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>17</v>
@@ -2491,19 +2476,19 @@
         <v>57</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>22</v>
@@ -2518,7 +2503,7 @@
         <v>55</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>17</v>
@@ -2550,32 +2535,32 @@
         <v>59</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>17</v>
@@ -2607,19 +2592,19 @@
         <v>61</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>22</v>
@@ -2632,7 +2617,7 @@
         <v>64</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>17</v>
@@ -2664,32 +2649,32 @@
         <v>65</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>17</v>
@@ -2721,19 +2706,19 @@
         <v>68</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>22</v>
@@ -2746,7 +2731,7 @@
         <v>30</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>17</v>
@@ -2778,32 +2763,32 @@
         <v>69</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>17</v>
@@ -2835,19 +2820,19 @@
         <v>71</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>22</v>
@@ -2860,7 +2845,7 @@
         <v>74</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>17</v>
@@ -2892,19 +2877,19 @@
         <v>71</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>22</v>
@@ -2917,7 +2902,7 @@
         <v>74</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>17</v>
@@ -2949,19 +2934,19 @@
         <v>77</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>22</v>
@@ -2976,7 +2961,7 @@
         <v>74</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>17</v>
@@ -3008,19 +2993,19 @@
         <v>77</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>22</v>
@@ -3035,7 +3020,7 @@
         <v>74</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>17</v>
@@ -3067,25 +3052,25 @@
         <v>81</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>38</v>
@@ -3094,7 +3079,7 @@
         <v>24</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>17</v>
@@ -3126,32 +3111,32 @@
         <v>82</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="5" t="s">
         <v>16</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>17</v>
@@ -3183,19 +3168,19 @@
         <v>84</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>22</v>
@@ -3208,7 +3193,7 @@
         <v>87</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>17</v>
@@ -3240,19 +3225,19 @@
         <v>88</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>22</v>
@@ -3265,7 +3250,7 @@
         <v>16</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>17</v>
@@ -3297,19 +3282,19 @@
         <v>90</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>22</v>
@@ -3322,7 +3307,7 @@
         <v>30</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>17</v>
@@ -3354,19 +3339,19 @@
         <v>91</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>22</v>
@@ -3379,7 +3364,7 @@
         <v>39</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>17</v>
@@ -3411,19 +3396,19 @@
         <v>93</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>22</v>
@@ -3438,7 +3423,7 @@
         <v>64</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>17</v>
@@ -3470,19 +3455,19 @@
         <v>93</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>22</v>
@@ -3497,7 +3482,7 @@
         <v>16</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>17</v>
@@ -3529,19 +3514,19 @@
         <v>96</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>22</v>
@@ -3578,19 +3563,19 @@
         <v>99</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>22</v>
@@ -3627,19 +3612,19 @@
         <v>101</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>22</v>
@@ -3652,7 +3637,7 @@
         <v>104</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>17</v>
@@ -3684,25 +3669,25 @@
         <v>105</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>231</v>
+        <v>362</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>230</v>
+        <v>361</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>79</v>
@@ -3711,7 +3696,7 @@
         <v>74</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>17</v>
@@ -3743,25 +3728,25 @@
         <v>105</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>231</v>
+        <v>362</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>230</v>
+        <v>361</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>79</v>
@@ -3770,7 +3755,7 @@
         <v>74</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>17</v>
@@ -3802,25 +3787,25 @@
         <v>107</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>231</v>
+        <v>362</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>230</v>
+        <v>361</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>79</v>
@@ -3829,7 +3814,7 @@
         <v>74</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>17</v>
@@ -3861,25 +3846,25 @@
         <v>107</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>231</v>
+        <v>362</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>230</v>
+        <v>361</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>79</v>
@@ -3888,7 +3873,7 @@
         <v>74</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>17</v>
@@ -3920,19 +3905,19 @@
         <v>108</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>110</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>22</v>
@@ -3947,7 +3932,7 @@
         <v>112</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>17</v>
@@ -3979,19 +3964,19 @@
         <v>113</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>22</v>
@@ -4004,7 +3989,7 @@
         <v>74</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>17</v>
@@ -4036,19 +4021,19 @@
         <v>113</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>114</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>22</v>
@@ -4061,7 +4046,7 @@
         <v>74</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>17</v>
@@ -4093,13 +4078,13 @@
         <v>115</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>117</v>
@@ -4140,13 +4125,13 @@
         <v>118</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>117</v>
@@ -4187,13 +4172,13 @@
         <v>120</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>122</v>
@@ -4234,19 +4219,19 @@
         <v>123</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>22</v>
@@ -4259,7 +4244,7 @@
         <v>74</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>17</v>
@@ -4291,19 +4276,19 @@
         <v>123</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>22</v>
@@ -4316,7 +4301,7 @@
         <v>74</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>17</v>
@@ -4348,13 +4333,13 @@
         <v>124</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>117</v>
@@ -4395,13 +4380,13 @@
         <v>125</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>117</v>
@@ -4442,19 +4427,19 @@
         <v>126</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>127</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>128</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>22</v>
@@ -4493,13 +4478,13 @@
         <v>129</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>130</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>122</v>
@@ -4542,7 +4527,7 @@
         <v>132</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>109</v>
@@ -4554,7 +4539,7 @@
         <v>134</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>22</v>
@@ -4569,7 +4554,7 @@
         <v>136</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>17</v>
@@ -4601,7 +4586,7 @@
         <v>132</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>109</v>
@@ -4613,7 +4598,7 @@
         <v>137</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>22</v>
@@ -4652,7 +4637,7 @@
         <v>132</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>109</v>
@@ -4664,7 +4649,7 @@
         <v>138</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>22</v>
@@ -4703,7 +4688,7 @@
         <v>132</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>109</v>
@@ -4715,7 +4700,7 @@
         <v>139</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>22</v>
@@ -4754,19 +4739,19 @@
         <v>140</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>141</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>142</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G59" s="8" t="s">
         <v>22</v>
@@ -4779,7 +4764,7 @@
         <v>143</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L59" s="8" t="s">
         <v>17</v>
@@ -4811,19 +4796,19 @@
         <v>140</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>141</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>144</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>22</v>
@@ -4836,7 +4821,7 @@
         <v>143</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>17</v>
@@ -4868,19 +4853,19 @@
         <v>145</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>146</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>128</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>22</v>
@@ -4917,19 +4902,19 @@
         <v>147</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>148</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>22</v>
@@ -4966,13 +4951,13 @@
         <v>150</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>151</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>152</v>
@@ -5015,19 +5000,19 @@
         <v>154</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>155</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>53</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>22</v>
@@ -5040,7 +5025,7 @@
         <v>156</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L64" s="8" t="s">
         <v>17</v>
@@ -5072,25 +5057,25 @@
         <v>157</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>158</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I65" s="7"/>
       <c r="J65" s="5"/>
@@ -5121,21 +5106,25 @@
         <v>160</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>161</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>234</v>
+        <v>286</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="I66" s="7"/>
       <c r="J66" s="5"/>
@@ -5166,19 +5155,19 @@
         <v>162</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>164</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>22</v>
@@ -5215,19 +5204,19 @@
         <v>165</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>166</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>167</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>22</v>
@@ -5264,7 +5253,7 @@
         <v>168</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>109</v>
@@ -5276,7 +5265,7 @@
         <v>134</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G69" s="8" t="s">
         <v>22</v>
@@ -5289,7 +5278,7 @@
         <v>136</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L69" s="8" t="s">
         <v>17</v>
@@ -5321,7 +5310,7 @@
         <v>168</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>109</v>
@@ -5333,7 +5322,7 @@
         <v>137</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G70" s="8" t="s">
         <v>22</v>
@@ -5370,7 +5359,7 @@
         <v>168</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>109</v>
@@ -5382,7 +5371,7 @@
         <v>138</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G71" s="8" t="s">
         <v>22</v>
@@ -5419,7 +5408,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>109</v>
@@ -5431,7 +5420,7 @@
         <v>139</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G72" s="8" t="s">
         <v>22</v>
@@ -5468,19 +5457,19 @@
         <v>169</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>170</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>171</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="G73" s="8" t="s">
         <v>22</v>
@@ -5493,7 +5482,7 @@
         <v>143</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L73" s="8" t="s">
         <v>17</v>
@@ -5525,32 +5514,32 @@
         <v>172</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I74" s="7"/>
       <c r="J74" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L74" s="8" t="s">
         <v>17</v>
@@ -5582,32 +5571,32 @@
         <v>172</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I75" s="7"/>
       <c r="J75" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L75" s="8" t="s">
         <v>17</v>
@@ -5639,25 +5628,25 @@
         <v>172</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>174</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I76" s="7"/>
       <c r="J76" s="5"/>
@@ -5688,32 +5677,32 @@
         <v>175</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I77" s="7"/>
       <c r="J77" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L77" s="8" t="s">
         <v>17</v>
@@ -5745,32 +5734,32 @@
         <v>175</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H78" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I78" s="7"/>
       <c r="J78" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L78" s="8" t="s">
         <v>17</v>
@@ -5802,32 +5791,32 @@
         <v>175</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I79" s="7"/>
       <c r="J79" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L79" s="8" t="s">
         <v>17</v>
@@ -5859,32 +5848,32 @@
         <v>175</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H80" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I80" s="7"/>
       <c r="J80" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L80" s="8" t="s">
         <v>17</v>
@@ -5916,25 +5905,25 @@
         <v>178</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>176</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I81" s="7" t="s">
         <v>179</v>
@@ -5943,7 +5932,7 @@
         <v>24</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L81" s="8" t="s">
         <v>17</v>
@@ -5975,32 +5964,32 @@
         <v>180</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>173</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H82" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L82" s="8" t="s">
         <v>17</v>
@@ -6032,32 +6021,32 @@
         <v>180</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>173</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G83" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>17</v>
@@ -6089,32 +6078,32 @@
         <v>180</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>181</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L84" s="8" t="s">
         <v>17</v>
@@ -6146,32 +6135,32 @@
         <v>180</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>181</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G85" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H85" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I85" s="7"/>
       <c r="J85" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L85" s="8" t="s">
         <v>17</v>
@@ -6203,32 +6192,32 @@
         <v>182</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I86" s="7"/>
       <c r="J86" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L86" s="8" t="s">
         <v>17</v>
@@ -6260,32 +6249,32 @@
         <v>182</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>173</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H87" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I87" s="13"/>
       <c r="J87" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L87" s="8" t="s">
         <v>17</v>
@@ -6317,25 +6306,25 @@
         <v>182</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>181</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H88" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I88" s="7"/>
       <c r="J88" s="5"/>
@@ -6366,32 +6355,32 @@
         <v>183</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C89" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G89" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I89" s="7"/>
       <c r="J89" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L89" s="8" t="s">
         <v>17</v>
@@ -6425,32 +6414,32 @@
         <v>183</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G90" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H90" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I90" s="7"/>
       <c r="J90" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L90" s="8" t="s">
         <v>17</v>
@@ -6484,25 +6473,25 @@
         <v>183</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>181</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G91" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I91" s="7"/>
       <c r="J91" s="5"/>
@@ -6535,32 +6524,32 @@
         <v>184</v>
       </c>
       <c r="B92" s="17" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>185</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G92" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H92" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I92" s="7"/>
       <c r="J92" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L92" s="8" t="s">
         <v>17</v>
@@ -6592,32 +6581,32 @@
         <v>184</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>185</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I93" s="7"/>
       <c r="J93" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L93" s="8" t="s">
         <v>17</v>
@@ -6649,25 +6638,25 @@
         <v>184</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>181</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G94" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H94" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I94" s="7"/>
       <c r="J94" s="5"/>
@@ -6698,32 +6687,32 @@
         <v>186</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G95" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H95" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K95" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L95" s="8" t="s">
         <v>17</v>
@@ -6755,32 +6744,32 @@
         <v>186</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C96" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G96" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K96" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L96" s="8" t="s">
         <v>17</v>
@@ -6812,32 +6801,32 @@
         <v>186</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C97" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G97" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L97" s="8" t="s">
         <v>17</v>
@@ -6869,32 +6858,32 @@
         <v>186</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G98" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H98" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I98" s="7"/>
       <c r="J98" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K98" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L98" s="8" t="s">
         <v>17</v>
@@ -6926,19 +6915,19 @@
         <v>187</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>189</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G99" s="8" t="s">
         <v>22</v>
@@ -6953,7 +6942,7 @@
         <v>112</v>
       </c>
       <c r="K99" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L99" s="8" t="s">
         <v>17</v>
@@ -6987,19 +6976,19 @@
         <v>191</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G100" s="8" t="s">
         <v>22</v>
@@ -7014,7 +7003,7 @@
         <v>104</v>
       </c>
       <c r="K100" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="L100" s="8" t="s">
         <v>17</v>
@@ -7046,19 +7035,19 @@
         <v>193</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G101" s="8" t="s">
         <v>22</v>
@@ -7071,7 +7060,7 @@
         <v>104</v>
       </c>
       <c r="K101" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="L101" s="8" t="s">
         <v>17</v>
@@ -7103,19 +7092,19 @@
         <v>194</v>
       </c>
       <c r="B102" s="17" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>195</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>196</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="G102" s="8" t="s">
         <v>22</v>
@@ -7152,7 +7141,7 @@
         <v>197</v>
       </c>
       <c r="B103" s="17" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
@@ -7160,7 +7149,7 @@
         <v>198</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G103" s="8" t="s">
         <v>22</v>
@@ -7197,19 +7186,19 @@
         <v>199</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C104" s="11" t="s">
         <v>200</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>159</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>22</v>
@@ -7246,19 +7235,19 @@
         <v>201</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>202</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>202</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>22</v>
@@ -7297,7 +7286,7 @@
         <v>204</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -7336,19 +7325,19 @@
         <v>206</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>202</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>202</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G107" s="8" t="s">
         <v>22</v>
@@ -7387,13 +7376,13 @@
         <v>208</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>209</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
@@ -7430,19 +7419,19 @@
         <v>211</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>212</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>213</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="G109" s="8" t="s">
         <v>22</v>
@@ -7479,32 +7468,32 @@
         <v>214</v>
       </c>
       <c r="B110" s="17" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C110" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G110" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I110" s="7"/>
       <c r="J110" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L110" s="8" t="s">
         <v>17</v>
@@ -7536,32 +7525,32 @@
         <v>214</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C111" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G111" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I111" s="7"/>
       <c r="J111" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L111" s="8" t="s">
         <v>17</v>
@@ -7593,32 +7582,32 @@
         <v>214</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C112" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G112" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I112" s="7"/>
       <c r="J112" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K112" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L112" s="8" t="s">
         <v>17</v>
@@ -7650,32 +7639,32 @@
         <v>214</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C113" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G113" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I113" s="7"/>
       <c r="J113" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L113" s="8" t="s">
         <v>17</v>
@@ -7707,7 +7696,7 @@
         <v>215</v>
       </c>
       <c r="B114" s="17" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
@@ -7715,7 +7704,7 @@
         <v>42</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G114" s="8" t="s">
         <v>22</v>
@@ -7728,7 +7717,7 @@
         <v>24</v>
       </c>
       <c r="K114" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L114" s="8" t="s">
         <v>17</v>
@@ -7760,7 +7749,7 @@
         <v>215</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
@@ -7768,7 +7757,7 @@
         <v>42</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G115" s="8" t="s">
         <v>22</v>
@@ -7781,7 +7770,7 @@
         <v>16</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L115" s="8" t="s">
         <v>17</v>
@@ -7813,7 +7802,7 @@
         <v>215</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
@@ -7821,7 +7810,7 @@
         <v>44</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G116" s="8" t="s">
         <v>22</v>
@@ -7834,7 +7823,7 @@
         <v>24</v>
       </c>
       <c r="K116" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L116" s="8" t="s">
         <v>17</v>
@@ -7866,7 +7855,7 @@
         <v>215</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
@@ -7874,7 +7863,7 @@
         <v>44</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G117" s="8" t="s">
         <v>22</v>
@@ -7887,7 +7876,7 @@
         <v>16</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L117" s="8" t="s">
         <v>17</v>
@@ -7919,7 +7908,7 @@
         <v>216</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
@@ -7927,7 +7916,7 @@
         <v>42</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G118" s="8" t="s">
         <v>22</v>
@@ -7942,7 +7931,7 @@
         <v>24</v>
       </c>
       <c r="K118" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L118" s="8" t="s">
         <v>17</v>
@@ -7974,7 +7963,7 @@
         <v>216</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C119" s="11"/>
       <c r="D119" s="11"/>
@@ -7982,7 +7971,7 @@
         <v>42</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G119" s="8" t="s">
         <v>22</v>
@@ -7997,7 +7986,7 @@
         <v>16</v>
       </c>
       <c r="K119" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L119" s="8" t="s">
         <v>17</v>
@@ -8029,7 +8018,7 @@
         <v>216</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C120" s="11"/>
       <c r="D120" s="11"/>
@@ -8037,7 +8026,7 @@
         <v>44</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G120" s="8" t="s">
         <v>22</v>
@@ -8052,7 +8041,7 @@
         <v>24</v>
       </c>
       <c r="K120" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L120" s="8" t="s">
         <v>17</v>
@@ -8084,7 +8073,7 @@
         <v>216</v>
       </c>
       <c r="B121" s="17" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
@@ -8092,7 +8081,7 @@
         <v>44</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G121" s="8" t="s">
         <v>22</v>
@@ -8107,7 +8096,7 @@
         <v>16</v>
       </c>
       <c r="K121" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L121" s="8" t="s">
         <v>17</v>
@@ -8139,25 +8128,25 @@
         <v>218</v>
       </c>
       <c r="B122" s="17" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C122" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G122" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I122" s="7" t="s">
         <v>217</v>
@@ -8166,7 +8155,7 @@
         <v>24</v>
       </c>
       <c r="K122" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L122" s="8" t="s">
         <v>17</v>
@@ -8198,25 +8187,25 @@
         <v>218</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C123" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G123" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I123" s="7" t="s">
         <v>217</v>
@@ -8225,7 +8214,7 @@
         <v>16</v>
       </c>
       <c r="K123" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L123" s="8" t="s">
         <v>17</v>
@@ -8257,25 +8246,25 @@
         <v>218</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C124" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G124" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I124" s="7" t="s">
         <v>217</v>
@@ -8284,7 +8273,7 @@
         <v>24</v>
       </c>
       <c r="K124" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L124" s="8" t="s">
         <v>17</v>
@@ -8316,25 +8305,25 @@
         <v>218</v>
       </c>
       <c r="B125" s="17" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C125" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G125" s="17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I125" s="7" t="s">
         <v>217</v>
@@ -8343,7 +8332,7 @@
         <v>16</v>
       </c>
       <c r="K125" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="L125" s="8" t="s">
         <v>17</v>
@@ -8370,33 +8359,21 @@
       <c r="AB125" s="5"/>
       <c r="AC125" s="5"/>
     </row>
-    <row r="126" spans="1:29" ht="15" x14ac:dyDescent="0.15">
-      <c r="A126" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B126" s="17" t="s">
-        <v>366</v>
-      </c>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F126" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="G126" s="8"/>
-      <c r="H126" s="8"/>
-      <c r="I126" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J126" s="8"/>
+    <row r="126" spans="1:29" ht="14" x14ac:dyDescent="0.15">
+      <c r="A126" s="5"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="7"/>
+      <c r="J126" s="5"/>
       <c r="K126" s="5"/>
       <c r="L126" s="5"/>
       <c r="M126" s="5"/>
-      <c r="N126" s="6">
-        <v>32637352</v>
-      </c>
+      <c r="N126" s="5"/>
       <c r="O126" s="5"/>
       <c r="P126" s="5"/>
       <c r="Q126" s="5"/>
@@ -37026,37 +37003,6 @@
       <c r="AB1049" s="5"/>
       <c r="AC1049" s="5"/>
     </row>
-    <row r="1050" spans="1:29" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1050" s="5"/>
-      <c r="B1050" s="17"/>
-      <c r="C1050" s="7"/>
-      <c r="D1050" s="7"/>
-      <c r="E1050" s="5"/>
-      <c r="F1050" s="5"/>
-      <c r="G1050" s="5"/>
-      <c r="H1050" s="5"/>
-      <c r="I1050" s="7"/>
-      <c r="J1050" s="5"/>
-      <c r="K1050" s="5"/>
-      <c r="L1050" s="5"/>
-      <c r="M1050" s="5"/>
-      <c r="N1050" s="5"/>
-      <c r="O1050" s="5"/>
-      <c r="P1050" s="5"/>
-      <c r="Q1050" s="5"/>
-      <c r="R1050" s="5"/>
-      <c r="S1050" s="5"/>
-      <c r="T1050" s="5"/>
-      <c r="U1050" s="5"/>
-      <c r="V1050" s="5"/>
-      <c r="W1050" s="5"/>
-      <c r="X1050" s="5"/>
-      <c r="Y1050" s="5"/>
-      <c r="Z1050" s="5"/>
-      <c r="AA1050" s="5"/>
-      <c r="AB1050" s="5"/>
-      <c r="AC1050" s="5"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Jinyang Du's drug-viral protein interaction annotation data incorporated to CIDO
Jinyang Du's drug-viral protein interaction annotation data incorporated to CIDO
- updated ontorat data file
- updated ontorat output files: Du_drug_Ontorat.owl, and Du_viral_Ontorat.owl
- updated CHEBI ontofox input and output files.
- updated cido-base.owl file.
</commit_message>
<xml_diff>
--- a/src/ontology/Ontorat input/Jinyang Du Ontorat/Du_reorganized_data.xlsx
+++ b/src/ontology/Ontorat input/Jinyang Du Ontorat/Du_reorganized_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA1BCC-5582-3543-93B7-071CFBF2FAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F16B77-7AF8-EA41-81DA-29E5CD75B1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Sheet" sheetId="1" r:id="rId1"/>
@@ -722,9 +722,6 @@
     <t>chemical binds protein</t>
   </si>
   <si>
-    <t>CHEBI_138090 </t>
-  </si>
-  <si>
     <t>ChEBI ID with Prefix</t>
   </si>
   <si>
@@ -1123,6 +1120,9 @@
   <si>
     <t>chemical degrades protein</t>
   </si>
+  <si>
+    <t>CHEBI_138090</t>
+  </si>
 </sst>
 </file>
 
@@ -1484,9 +1484,9 @@
   </sheetPr>
   <dimension ref="A1:AC1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1509,10 +1509,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1572,19 +1572,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>14</v>
@@ -1597,7 +1597,7 @@
         <v>16</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>17</v>
@@ -1629,19 +1629,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>229</v>
+        <v>362</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>22</v>
@@ -1654,7 +1654,7 @@
         <v>24</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>17</v>
@@ -1686,19 +1686,19 @@
         <v>19</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>229</v>
+        <v>362</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>22</v>
@@ -1711,7 +1711,7 @@
         <v>25</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>17</v>
@@ -1743,19 +1743,19 @@
         <v>19</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>229</v>
+        <v>362</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>22</v>
@@ -1792,19 +1792,19 @@
         <v>27</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>22</v>
@@ -1817,7 +1817,7 @@
         <v>30</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>17</v>
@@ -1849,19 +1849,19 @@
         <v>31</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>22</v>
@@ -1874,7 +1874,7 @@
         <v>34</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>17</v>
@@ -1906,19 +1906,19 @@
         <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>22</v>
@@ -1933,7 +1933,7 @@
         <v>39</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>17</v>
@@ -1969,19 +1969,19 @@
         <v>40</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>226</v>
@@ -1994,7 +1994,7 @@
         <v>24</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>17</v>
@@ -2028,19 +2028,19 @@
         <v>40</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>226</v>
@@ -2053,7 +2053,7 @@
         <v>16</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>17</v>
@@ -2087,19 +2087,19 @@
         <v>40</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>227</v>
@@ -2138,19 +2138,19 @@
         <v>45</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>14</v>
@@ -2163,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>17</v>
@@ -2195,19 +2195,19 @@
         <v>45</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>14</v>
@@ -2220,7 +2220,7 @@
         <v>16</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>17</v>
@@ -2252,19 +2252,19 @@
         <v>45</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>14</v>
@@ -2301,19 +2301,19 @@
         <v>48</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>22</v>
@@ -2326,7 +2326,7 @@
         <v>16</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>17</v>
@@ -2358,19 +2358,19 @@
         <v>51</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>22</v>
@@ -2385,7 +2385,7 @@
         <v>55</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>17</v>
@@ -2417,19 +2417,19 @@
         <v>51</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>22</v>
@@ -2444,7 +2444,7 @@
         <v>55</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>17</v>
@@ -2476,19 +2476,19 @@
         <v>57</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>22</v>
@@ -2503,7 +2503,7 @@
         <v>55</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>17</v>
@@ -2535,19 +2535,19 @@
         <v>59</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>226</v>
@@ -2560,7 +2560,7 @@
         <v>24</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>17</v>
@@ -2592,19 +2592,19 @@
         <v>61</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>22</v>
@@ -2617,7 +2617,7 @@
         <v>64</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>17</v>
@@ -2649,19 +2649,19 @@
         <v>65</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>226</v>
@@ -2674,7 +2674,7 @@
         <v>24</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>17</v>
@@ -2706,19 +2706,19 @@
         <v>68</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>22</v>
@@ -2731,7 +2731,7 @@
         <v>30</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>17</v>
@@ -2763,19 +2763,19 @@
         <v>69</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>227</v>
@@ -2788,7 +2788,7 @@
         <v>24</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>17</v>
@@ -2820,19 +2820,19 @@
         <v>71</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>22</v>
@@ -2845,7 +2845,7 @@
         <v>74</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>17</v>
@@ -2877,19 +2877,19 @@
         <v>71</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>75</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>22</v>
@@ -2902,7 +2902,7 @@
         <v>74</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>17</v>
@@ -2934,19 +2934,19 @@
         <v>77</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>22</v>
@@ -2961,7 +2961,7 @@
         <v>74</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>17</v>
@@ -2993,19 +2993,19 @@
         <v>77</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>22</v>
@@ -3020,7 +3020,7 @@
         <v>74</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>17</v>
@@ -3052,19 +3052,19 @@
         <v>81</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>226</v>
@@ -3079,7 +3079,7 @@
         <v>24</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>17</v>
@@ -3111,19 +3111,19 @@
         <v>82</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>227</v>
@@ -3136,7 +3136,7 @@
         <v>16</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>17</v>
@@ -3168,19 +3168,19 @@
         <v>84</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>22</v>
@@ -3193,7 +3193,7 @@
         <v>87</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>17</v>
@@ -3225,19 +3225,19 @@
         <v>88</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>22</v>
@@ -3250,7 +3250,7 @@
         <v>16</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>17</v>
@@ -3282,19 +3282,19 @@
         <v>90</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>22</v>
@@ -3307,7 +3307,7 @@
         <v>30</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>17</v>
@@ -3339,19 +3339,19 @@
         <v>91</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>22</v>
@@ -3364,7 +3364,7 @@
         <v>39</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>17</v>
@@ -3396,19 +3396,19 @@
         <v>93</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>22</v>
@@ -3423,7 +3423,7 @@
         <v>64</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>17</v>
@@ -3455,19 +3455,19 @@
         <v>93</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>22</v>
@@ -3482,7 +3482,7 @@
         <v>16</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L35" s="8" t="s">
         <v>17</v>
@@ -3514,19 +3514,19 @@
         <v>96</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>22</v>
@@ -3563,19 +3563,19 @@
         <v>99</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>22</v>
@@ -3612,19 +3612,19 @@
         <v>101</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>22</v>
@@ -3637,7 +3637,7 @@
         <v>104</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>17</v>
@@ -3669,25 +3669,25 @@
         <v>105</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>79</v>
@@ -3696,7 +3696,7 @@
         <v>74</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L39" s="8" t="s">
         <v>17</v>
@@ -3728,25 +3728,25 @@
         <v>105</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>79</v>
@@ -3755,7 +3755,7 @@
         <v>74</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>17</v>
@@ -3787,25 +3787,25 @@
         <v>107</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>79</v>
@@ -3814,7 +3814,7 @@
         <v>74</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L41" s="8" t="s">
         <v>17</v>
@@ -3846,25 +3846,25 @@
         <v>107</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>79</v>
@@ -3873,7 +3873,7 @@
         <v>74</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>17</v>
@@ -3905,13 +3905,13 @@
         <v>108</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>110</v>
@@ -3932,7 +3932,7 @@
         <v>112</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>17</v>
@@ -3964,19 +3964,19 @@
         <v>113</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>22</v>
@@ -3989,7 +3989,7 @@
         <v>74</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>17</v>
@@ -4021,19 +4021,19 @@
         <v>113</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>114</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>22</v>
@@ -4046,7 +4046,7 @@
         <v>74</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>17</v>
@@ -4078,13 +4078,13 @@
         <v>115</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>117</v>
@@ -4125,13 +4125,13 @@
         <v>118</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>117</v>
@@ -4172,13 +4172,13 @@
         <v>120</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>122</v>
@@ -4219,19 +4219,19 @@
         <v>123</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>73</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>22</v>
@@ -4244,7 +4244,7 @@
         <v>74</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>17</v>
@@ -4276,19 +4276,19 @@
         <v>123</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>76</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>22</v>
@@ -4301,7 +4301,7 @@
         <v>74</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L50" s="8" t="s">
         <v>17</v>
@@ -4333,13 +4333,13 @@
         <v>124</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>119</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>117</v>
@@ -4380,13 +4380,13 @@
         <v>125</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>117</v>
@@ -4427,19 +4427,19 @@
         <v>126</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>127</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>128</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>22</v>
@@ -4478,13 +4478,13 @@
         <v>129</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>130</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>122</v>
@@ -4554,7 +4554,7 @@
         <v>136</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>17</v>
@@ -4598,7 +4598,7 @@
         <v>137</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>22</v>
@@ -4649,7 +4649,7 @@
         <v>138</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>22</v>
@@ -4700,7 +4700,7 @@
         <v>139</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>22</v>
@@ -4739,19 +4739,19 @@
         <v>140</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>141</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>142</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G59" s="8" t="s">
         <v>22</v>
@@ -4796,19 +4796,19 @@
         <v>140</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>141</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>144</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>22</v>
@@ -4853,19 +4853,19 @@
         <v>145</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>146</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>128</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>22</v>
@@ -4902,19 +4902,19 @@
         <v>147</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>148</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>22</v>
@@ -4951,13 +4951,13 @@
         <v>150</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>151</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>152</v>
@@ -5000,19 +5000,19 @@
         <v>154</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>155</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>53</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>22</v>
@@ -5025,7 +5025,7 @@
         <v>156</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L64" s="8" t="s">
         <v>17</v>
@@ -5057,19 +5057,19 @@
         <v>157</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>158</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>159</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>228</v>
@@ -5106,19 +5106,19 @@
         <v>160</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>161</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>128</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G66" s="17" t="s">
         <v>22</v>
@@ -5155,19 +5155,19 @@
         <v>162</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>164</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>22</v>
@@ -5204,19 +5204,19 @@
         <v>165</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>166</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>167</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>22</v>
@@ -5253,7 +5253,7 @@
         <v>168</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>109</v>
@@ -5278,7 +5278,7 @@
         <v>136</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L69" s="8" t="s">
         <v>17</v>
@@ -5310,7 +5310,7 @@
         <v>168</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>109</v>
@@ -5322,7 +5322,7 @@
         <v>137</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G70" s="8" t="s">
         <v>22</v>
@@ -5359,7 +5359,7 @@
         <v>168</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>109</v>
@@ -5371,7 +5371,7 @@
         <v>138</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G71" s="8" t="s">
         <v>22</v>
@@ -5408,7 +5408,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>109</v>
@@ -5420,7 +5420,7 @@
         <v>139</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G72" s="8" t="s">
         <v>22</v>
@@ -5457,19 +5457,19 @@
         <v>169</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>170</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>171</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G73" s="8" t="s">
         <v>22</v>
@@ -5514,19 +5514,19 @@
         <v>172</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G74" s="17" t="s">
         <v>227</v>
@@ -5539,7 +5539,7 @@
         <v>24</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L74" s="8" t="s">
         <v>17</v>
@@ -5571,19 +5571,19 @@
         <v>172</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G75" s="17" t="s">
         <v>227</v>
@@ -5596,7 +5596,7 @@
         <v>16</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L75" s="8" t="s">
         <v>17</v>
@@ -5628,19 +5628,19 @@
         <v>172</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>174</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G76" s="17" t="s">
         <v>227</v>
@@ -5677,19 +5677,19 @@
         <v>175</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G77" s="17" t="s">
         <v>228</v>
@@ -5702,7 +5702,7 @@
         <v>24</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L77" s="8" t="s">
         <v>17</v>
@@ -5734,19 +5734,19 @@
         <v>175</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G78" s="17" t="s">
         <v>228</v>
@@ -5759,7 +5759,7 @@
         <v>16</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L78" s="8" t="s">
         <v>17</v>
@@ -5791,19 +5791,19 @@
         <v>175</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G79" s="17" t="s">
         <v>228</v>
@@ -5816,7 +5816,7 @@
         <v>24</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L79" s="8" t="s">
         <v>17</v>
@@ -5848,19 +5848,19 @@
         <v>175</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G80" s="17" t="s">
         <v>228</v>
@@ -5873,7 +5873,7 @@
         <v>16</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L80" s="8" t="s">
         <v>17</v>
@@ -5905,19 +5905,19 @@
         <v>178</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>176</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G81" s="17" t="s">
         <v>228</v>
@@ -5932,7 +5932,7 @@
         <v>24</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L81" s="8" t="s">
         <v>17</v>
@@ -5964,19 +5964,19 @@
         <v>180</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>173</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G82" s="17" t="s">
         <v>227</v>
@@ -5989,7 +5989,7 @@
         <v>24</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L82" s="8" t="s">
         <v>17</v>
@@ -6021,19 +6021,19 @@
         <v>180</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>173</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G83" s="17" t="s">
         <v>227</v>
@@ -6046,7 +6046,7 @@
         <v>16</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L83" s="8" t="s">
         <v>17</v>
@@ -6078,19 +6078,19 @@
         <v>180</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>181</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G84" s="17" t="s">
         <v>228</v>
@@ -6103,7 +6103,7 @@
         <v>24</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L84" s="8" t="s">
         <v>17</v>
@@ -6135,19 +6135,19 @@
         <v>180</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>181</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G85" s="17" t="s">
         <v>228</v>
@@ -6160,7 +6160,7 @@
         <v>16</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L85" s="8" t="s">
         <v>17</v>
@@ -6192,19 +6192,19 @@
         <v>182</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G86" s="17" t="s">
         <v>227</v>
@@ -6217,7 +6217,7 @@
         <v>24</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L86" s="8" t="s">
         <v>17</v>
@@ -6249,19 +6249,19 @@
         <v>182</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>173</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E87" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G87" s="17" t="s">
         <v>227</v>
@@ -6274,7 +6274,7 @@
         <v>16</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L87" s="8" t="s">
         <v>17</v>
@@ -6306,19 +6306,19 @@
         <v>182</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>181</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G88" s="17" t="s">
         <v>228</v>
@@ -6355,19 +6355,19 @@
         <v>183</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C89" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G89" s="17" t="s">
         <v>227</v>
@@ -6380,7 +6380,7 @@
         <v>24</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L89" s="8" t="s">
         <v>17</v>
@@ -6414,19 +6414,19 @@
         <v>183</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>173</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G90" s="17" t="s">
         <v>227</v>
@@ -6439,7 +6439,7 @@
         <v>16</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L90" s="8" t="s">
         <v>17</v>
@@ -6473,19 +6473,19 @@
         <v>183</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>181</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G91" s="17" t="s">
         <v>228</v>
@@ -6524,19 +6524,19 @@
         <v>184</v>
       </c>
       <c r="B92" s="17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>185</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G92" s="17" t="s">
         <v>226</v>
@@ -6549,7 +6549,7 @@
         <v>24</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L92" s="8" t="s">
         <v>17</v>
@@ -6581,19 +6581,19 @@
         <v>184</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>185</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G93" s="17" t="s">
         <v>226</v>
@@ -6606,7 +6606,7 @@
         <v>16</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L93" s="8" t="s">
         <v>17</v>
@@ -6638,19 +6638,19 @@
         <v>184</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>181</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G94" s="17" t="s">
         <v>228</v>
@@ -6687,19 +6687,19 @@
         <v>186</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G95" s="17" t="s">
         <v>228</v>
@@ -6712,7 +6712,7 @@
         <v>24</v>
       </c>
       <c r="K95" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L95" s="8" t="s">
         <v>17</v>
@@ -6744,19 +6744,19 @@
         <v>186</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C96" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G96" s="17" t="s">
         <v>228</v>
@@ -6769,7 +6769,7 @@
         <v>16</v>
       </c>
       <c r="K96" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L96" s="8" t="s">
         <v>17</v>
@@ -6801,19 +6801,19 @@
         <v>186</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C97" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G97" s="17" t="s">
         <v>228</v>
@@ -6826,7 +6826,7 @@
         <v>24</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L97" s="8" t="s">
         <v>17</v>
@@ -6858,19 +6858,19 @@
         <v>186</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G98" s="17" t="s">
         <v>228</v>
@@ -6883,7 +6883,7 @@
         <v>16</v>
       </c>
       <c r="K98" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L98" s="8" t="s">
         <v>17</v>
@@ -6915,19 +6915,19 @@
         <v>187</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>188</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>189</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G99" s="8" t="s">
         <v>22</v>
@@ -6942,7 +6942,7 @@
         <v>112</v>
       </c>
       <c r="K99" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L99" s="8" t="s">
         <v>17</v>
@@ -6976,19 +6976,19 @@
         <v>191</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G100" s="8" t="s">
         <v>22</v>
@@ -7003,7 +7003,7 @@
         <v>104</v>
       </c>
       <c r="K100" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L100" s="8" t="s">
         <v>17</v>
@@ -7035,19 +7035,19 @@
         <v>193</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>103</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G101" s="8" t="s">
         <v>22</v>
@@ -7060,7 +7060,7 @@
         <v>104</v>
       </c>
       <c r="K101" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L101" s="8" t="s">
         <v>17</v>
@@ -7092,19 +7092,19 @@
         <v>194</v>
       </c>
       <c r="B102" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>195</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>196</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G102" s="8" t="s">
         <v>22</v>
@@ -7141,7 +7141,7 @@
         <v>197</v>
       </c>
       <c r="B103" s="17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
@@ -7149,7 +7149,7 @@
         <v>198</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G103" s="8" t="s">
         <v>22</v>
@@ -7186,19 +7186,19 @@
         <v>199</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C104" s="11" t="s">
         <v>200</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>159</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>22</v>
@@ -7235,19 +7235,19 @@
         <v>201</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>202</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>202</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>22</v>
@@ -7286,7 +7286,7 @@
         <v>204</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
@@ -7325,19 +7325,19 @@
         <v>206</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>202</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>202</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G107" s="8" t="s">
         <v>22</v>
@@ -7376,13 +7376,13 @@
         <v>208</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>209</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
@@ -7419,19 +7419,19 @@
         <v>211</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>212</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>213</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G109" s="8" t="s">
         <v>22</v>
@@ -7468,19 +7468,19 @@
         <v>214</v>
       </c>
       <c r="B110" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C110" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G110" s="17" t="s">
         <v>228</v>
@@ -7493,7 +7493,7 @@
         <v>24</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L110" s="8" t="s">
         <v>17</v>
@@ -7525,19 +7525,19 @@
         <v>214</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C111" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G111" s="17" t="s">
         <v>228</v>
@@ -7550,7 +7550,7 @@
         <v>16</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L111" s="8" t="s">
         <v>17</v>
@@ -7582,19 +7582,19 @@
         <v>214</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C112" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G112" s="17" t="s">
         <v>228</v>
@@ -7607,7 +7607,7 @@
         <v>24</v>
       </c>
       <c r="K112" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L112" s="8" t="s">
         <v>17</v>
@@ -7639,19 +7639,19 @@
         <v>214</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C113" s="11" t="s">
         <v>177</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G113" s="17" t="s">
         <v>228</v>
@@ -7664,7 +7664,7 @@
         <v>16</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L113" s="8" t="s">
         <v>17</v>
@@ -7696,7 +7696,7 @@
         <v>215</v>
       </c>
       <c r="B114" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
@@ -7704,7 +7704,7 @@
         <v>42</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G114" s="8" t="s">
         <v>22</v>
@@ -7717,7 +7717,7 @@
         <v>24</v>
       </c>
       <c r="K114" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L114" s="8" t="s">
         <v>17</v>
@@ -7749,7 +7749,7 @@
         <v>215</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
@@ -7757,7 +7757,7 @@
         <v>42</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G115" s="8" t="s">
         <v>22</v>
@@ -7770,7 +7770,7 @@
         <v>16</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L115" s="8" t="s">
         <v>17</v>
@@ -7802,7 +7802,7 @@
         <v>215</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
@@ -7810,7 +7810,7 @@
         <v>44</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G116" s="8" t="s">
         <v>22</v>
@@ -7823,7 +7823,7 @@
         <v>24</v>
       </c>
       <c r="K116" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L116" s="8" t="s">
         <v>17</v>
@@ -7855,7 +7855,7 @@
         <v>215</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
@@ -7863,7 +7863,7 @@
         <v>44</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G117" s="8" t="s">
         <v>22</v>
@@ -7876,7 +7876,7 @@
         <v>16</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L117" s="8" t="s">
         <v>17</v>
@@ -7908,7 +7908,7 @@
         <v>216</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
@@ -7916,7 +7916,7 @@
         <v>42</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G118" s="8" t="s">
         <v>22</v>
@@ -7931,7 +7931,7 @@
         <v>24</v>
       </c>
       <c r="K118" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L118" s="8" t="s">
         <v>17</v>
@@ -7963,7 +7963,7 @@
         <v>216</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C119" s="11"/>
       <c r="D119" s="11"/>
@@ -7971,7 +7971,7 @@
         <v>42</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G119" s="8" t="s">
         <v>22</v>
@@ -7986,7 +7986,7 @@
         <v>16</v>
       </c>
       <c r="K119" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L119" s="8" t="s">
         <v>17</v>
@@ -8018,7 +8018,7 @@
         <v>216</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C120" s="11"/>
       <c r="D120" s="11"/>
@@ -8026,7 +8026,7 @@
         <v>44</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G120" s="8" t="s">
         <v>22</v>
@@ -8041,7 +8041,7 @@
         <v>24</v>
       </c>
       <c r="K120" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L120" s="8" t="s">
         <v>17</v>
@@ -8073,7 +8073,7 @@
         <v>216</v>
       </c>
       <c r="B121" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
@@ -8081,7 +8081,7 @@
         <v>44</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G121" s="8" t="s">
         <v>22</v>
@@ -8096,7 +8096,7 @@
         <v>16</v>
       </c>
       <c r="K121" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L121" s="8" t="s">
         <v>17</v>
@@ -8128,19 +8128,19 @@
         <v>218</v>
       </c>
       <c r="B122" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C122" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G122" s="17" t="s">
         <v>226</v>
@@ -8155,7 +8155,7 @@
         <v>24</v>
       </c>
       <c r="K122" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L122" s="8" t="s">
         <v>17</v>
@@ -8187,19 +8187,19 @@
         <v>218</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C123" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G123" s="17" t="s">
         <v>226</v>
@@ -8214,7 +8214,7 @@
         <v>16</v>
       </c>
       <c r="K123" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L123" s="8" t="s">
         <v>17</v>
@@ -8246,19 +8246,19 @@
         <v>218</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C124" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G124" s="17" t="s">
         <v>226</v>
@@ -8273,7 +8273,7 @@
         <v>24</v>
       </c>
       <c r="K124" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L124" s="8" t="s">
         <v>17</v>
@@ -8305,19 +8305,19 @@
         <v>218</v>
       </c>
       <c r="B125" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C125" s="11" t="s">
         <v>219</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>44</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G125" s="17" t="s">
         <v>226</v>
@@ -8332,7 +8332,7 @@
         <v>16</v>
       </c>
       <c r="K125" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L125" s="8" t="s">
         <v>17</v>

</xml_diff>